<commit_message>
last sloppy commit, i promise
</commit_message>
<xml_diff>
--- a/tasks_db.xlsx
+++ b/tasks_db.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,19 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -435,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,38 +434,26 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2025-01-20</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Task 1</t>
+          <t>Tasks</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
-          <t>2025-01-20</t>
+          <t>2025-01-31</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Task 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>2025-01-20</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - Task 3</t>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>